<commit_message>
Plan, checklist and test cases updated
</commit_message>
<xml_diff>
--- a/Documentation/Check.xlsx
+++ b/Documentation/Check.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="208">
   <si>
     <t>Группа проверок/модуль</t>
   </si>
@@ -307,6 +307,9 @@
     <t>Выбрать завтрашнюю дату</t>
   </si>
   <si>
+    <t>Выбрать дату через месяц</t>
+  </si>
+  <si>
     <t>Выбрать дату через год</t>
   </si>
   <si>
@@ -343,7 +346,7 @@
     <t>Тап на кнопку Редактировать</t>
   </si>
   <si>
-    <t>Раздел редактирования новостей</t>
+    <t>Раздел Панель управления новостей</t>
   </si>
   <si>
     <t>Тап на Добавить новость</t>
@@ -418,7 +421,7 @@
     <t>Выбрать период с сегодняшнего дня и на неделю вперед</t>
   </si>
   <si>
-    <t>Выбрать период с завтрашного дня и до вчерашнего дня</t>
+    <t>Выбрать период с завтрашнего дня и до вчерашнего дня</t>
   </si>
   <si>
     <t>Отображается пустой список новостей, нет поп-апа с предупреждением</t>
@@ -451,6 +454,33 @@
     <t>Оставить оба поля даты пустыми</t>
   </si>
   <si>
+    <t>Редактирование новости</t>
+  </si>
+  <si>
+    <t>Изменить поле Категория на значение из выпадающего списка</t>
+  </si>
+  <si>
+    <t>Изменить поле Заголовок</t>
+  </si>
+  <si>
+    <t>Изменить поле Дата публикации</t>
+  </si>
+  <si>
+    <t>Изменить чек-бокс с активна на неактивна</t>
+  </si>
+  <si>
+    <t>Изменить чек-бокс с неактивна на активна</t>
+  </si>
+  <si>
+    <t>Изменить поле Категория на значение не из выпадающего списка</t>
+  </si>
+  <si>
+    <t>Текст снека не соответствует</t>
+  </si>
+  <si>
+    <t>Изменить новость и не сохранить</t>
+  </si>
+  <si>
     <t>Добавление новости</t>
   </si>
   <si>
@@ -464,9 +494,6 @@
   </si>
   <si>
     <t>Ввести в поле Категория значение не из списка</t>
-  </si>
-  <si>
-    <t>Текст снека не соответствует</t>
   </si>
   <si>
     <t>Выбрать вчерашнюю дату в Дате публикации</t>
@@ -614,7 +641,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="13">
+  <fonts count="12">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -662,10 +689,6 @@
     <font>
       <i/>
       <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <color rgb="FFFF0000"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -792,7 +815,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -842,11 +865,11 @@
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
     <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="6" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
@@ -855,9 +878,6 @@
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3615,7 +3635,7 @@
       <c r="W86" s="5"/>
     </row>
     <row r="87">
-      <c r="A87" s="14"/>
+      <c r="A87" s="13"/>
       <c r="B87" s="10" t="s">
         <v>104</v>
       </c>
@@ -3644,12 +3664,14 @@
       <c r="W87" s="5"/>
     </row>
     <row r="88">
-      <c r="A88" s="6" t="s">
+      <c r="A88" s="14"/>
+      <c r="B88" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="B88" s="7"/>
-      <c r="C88" s="7"/>
-      <c r="D88" s="8"/>
+      <c r="C88" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D88" s="12"/>
       <c r="E88" s="5"/>
       <c r="F88" s="5"/>
       <c r="G88" s="5"/>
@@ -3671,16 +3693,12 @@
       <c r="W88" s="5"/>
     </row>
     <row r="89">
-      <c r="A89" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B89" s="10" t="s">
+      <c r="A89" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="C89" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D89" s="12"/>
+      <c r="B89" s="7"/>
+      <c r="C89" s="7"/>
+      <c r="D89" s="8"/>
       <c r="E89" s="5"/>
       <c r="F89" s="5"/>
       <c r="G89" s="5"/>
@@ -3702,16 +3720,16 @@
       <c r="W89" s="5"/>
     </row>
     <row r="90">
-      <c r="A90" s="13"/>
+      <c r="A90" s="9" t="s">
+        <v>18</v>
+      </c>
       <c r="B90" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="C90" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D90" s="16" t="s">
-        <v>108</v>
-      </c>
+      <c r="C90" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D90" s="12"/>
       <c r="E90" s="5"/>
       <c r="F90" s="5"/>
       <c r="G90" s="5"/>
@@ -3735,12 +3753,14 @@
     <row r="91">
       <c r="A91" s="13"/>
       <c r="B91" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C91" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D91" s="12"/>
+        <v>108</v>
+      </c>
+      <c r="C91" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D91" s="16" t="s">
+        <v>109</v>
+      </c>
       <c r="E91" s="5"/>
       <c r="F91" s="5"/>
       <c r="G91" s="5"/>
@@ -3762,9 +3782,9 @@
       <c r="W91" s="5"/>
     </row>
     <row r="92">
-      <c r="A92" s="14"/>
+      <c r="A92" s="13"/>
       <c r="B92" s="10" t="s">
-        <v>109</v>
+        <v>40</v>
       </c>
       <c r="C92" s="11" t="s">
         <v>7</v>
@@ -3791,11 +3811,9 @@
       <c r="W92" s="5"/>
     </row>
     <row r="93">
-      <c r="A93" s="9" t="s">
+      <c r="A93" s="14"/>
+      <c r="B93" s="10" t="s">
         <v>110</v>
-      </c>
-      <c r="B93" s="10" t="s">
-        <v>111</v>
       </c>
       <c r="C93" s="11" t="s">
         <v>7</v>
@@ -3822,9 +3840,11 @@
       <c r="W93" s="5"/>
     </row>
     <row r="94">
-      <c r="A94" s="13"/>
+      <c r="A94" s="9" t="s">
+        <v>111</v>
+      </c>
       <c r="B94" s="10" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="C94" s="11" t="s">
         <v>7</v>
@@ -3853,7 +3873,7 @@
     <row r="95">
       <c r="A95" s="13"/>
       <c r="B95" s="10" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C95" s="11" t="s">
         <v>7</v>
@@ -3881,7 +3901,7 @@
     </row>
     <row r="96">
       <c r="A96" s="13"/>
-      <c r="B96" s="17" t="s">
+      <c r="B96" s="10" t="s">
         <v>113</v>
       </c>
       <c r="C96" s="11" t="s">
@@ -3910,7 +3930,7 @@
     </row>
     <row r="97">
       <c r="A97" s="13"/>
-      <c r="B97" s="10" t="s">
+      <c r="B97" s="17" t="s">
         <v>114</v>
       </c>
       <c r="C97" s="11" t="s">
@@ -3940,7 +3960,7 @@
     <row r="98">
       <c r="A98" s="13"/>
       <c r="B98" s="10" t="s">
-        <v>40</v>
+        <v>115</v>
       </c>
       <c r="C98" s="11" t="s">
         <v>7</v>
@@ -3967,9 +3987,9 @@
       <c r="W98" s="5"/>
     </row>
     <row r="99">
-      <c r="A99" s="14"/>
+      <c r="A99" s="13"/>
       <c r="B99" s="10" t="s">
-        <v>107</v>
+        <v>40</v>
       </c>
       <c r="C99" s="11" t="s">
         <v>7</v>
@@ -3996,16 +4016,14 @@
       <c r="W99" s="5"/>
     </row>
     <row r="100">
-      <c r="A100" s="9" t="s">
-        <v>115</v>
-      </c>
+      <c r="A100" s="14"/>
       <c r="B100" s="10" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C100" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D100" s="12"/>
+      <c r="D100" s="19"/>
       <c r="E100" s="5"/>
       <c r="F100" s="5"/>
       <c r="G100" s="5"/>
@@ -4027,7 +4045,9 @@
       <c r="W100" s="5"/>
     </row>
     <row r="101">
-      <c r="A101" s="13"/>
+      <c r="A101" s="9" t="s">
+        <v>116</v>
+      </c>
       <c r="B101" s="10" t="s">
         <v>117</v>
       </c>
@@ -4321,12 +4341,10 @@
       <c r="B111" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="C111" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D111" s="16" t="s">
-        <v>128</v>
-      </c>
+      <c r="C111" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D111" s="12"/>
       <c r="E111" s="5"/>
       <c r="F111" s="5"/>
       <c r="G111" s="5"/>
@@ -4348,14 +4366,16 @@
       <c r="W111" s="5"/>
     </row>
     <row r="112">
-      <c r="A112" s="14"/>
+      <c r="A112" s="13"/>
       <c r="B112" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="C112" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D112" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="C112" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D112" s="12"/>
       <c r="E112" s="5"/>
       <c r="F112" s="5"/>
       <c r="G112" s="5"/>
@@ -4377,18 +4397,14 @@
       <c r="W112" s="5"/>
     </row>
     <row r="113">
-      <c r="A113" s="9" t="s">
+      <c r="A113" s="14"/>
+      <c r="B113" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="B113" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="C113" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D113" s="16" t="s">
-        <v>128</v>
-      </c>
+      <c r="C113" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D113" s="12"/>
       <c r="E113" s="5"/>
       <c r="F113" s="5"/>
       <c r="G113" s="5"/>
@@ -4410,14 +4426,18 @@
       <c r="W113" s="5"/>
     </row>
     <row r="114">
-      <c r="A114" s="13"/>
+      <c r="A114" s="9" t="s">
+        <v>131</v>
+      </c>
       <c r="B114" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="C114" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D114" s="12"/>
+      <c r="C114" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D114" s="16" t="s">
+        <v>129</v>
+      </c>
       <c r="E114" s="5"/>
       <c r="F114" s="5"/>
       <c r="G114" s="5"/>
@@ -4501,12 +4521,10 @@
       <c r="B117" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="C117" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D117" s="16" t="s">
-        <v>136</v>
-      </c>
+      <c r="C117" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D117" s="12"/>
       <c r="E117" s="5"/>
       <c r="F117" s="5"/>
       <c r="G117" s="5"/>
@@ -4530,12 +4548,14 @@
     <row r="118">
       <c r="A118" s="13"/>
       <c r="B118" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="C118" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D118" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="C118" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D118" s="12"/>
       <c r="E118" s="5"/>
       <c r="F118" s="5"/>
       <c r="G118" s="5"/>
@@ -4561,12 +4581,10 @@
       <c r="B119" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="C119" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D119" s="16" t="s">
-        <v>139</v>
-      </c>
+      <c r="C119" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D119" s="12"/>
       <c r="E119" s="5"/>
       <c r="F119" s="5"/>
       <c r="G119" s="5"/>
@@ -4590,13 +4608,13 @@
     <row r="120">
       <c r="A120" s="13"/>
       <c r="B120" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C120" s="15" t="s">
         <v>13</v>
       </c>
       <c r="D120" s="16" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E120" s="5"/>
       <c r="F120" s="5"/>
@@ -4627,7 +4645,7 @@
         <v>13</v>
       </c>
       <c r="D121" s="16" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E121" s="5"/>
       <c r="F121" s="5"/>
@@ -4658,7 +4676,7 @@
         <v>13</v>
       </c>
       <c r="D122" s="16" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E122" s="5"/>
       <c r="F122" s="5"/>
@@ -4689,7 +4707,7 @@
         <v>13</v>
       </c>
       <c r="D123" s="16" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E123" s="5"/>
       <c r="F123" s="5"/>
@@ -4720,7 +4738,7 @@
         <v>13</v>
       </c>
       <c r="D124" s="16" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E124" s="5"/>
       <c r="F124" s="5"/>
@@ -4743,14 +4761,16 @@
       <c r="W124" s="5"/>
     </row>
     <row r="125">
-      <c r="A125" s="14"/>
+      <c r="A125" s="13"/>
       <c r="B125" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="C125" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D125" s="12"/>
+      <c r="C125" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D125" s="16" t="s">
+        <v>140</v>
+      </c>
       <c r="E125" s="5"/>
       <c r="F125" s="5"/>
       <c r="G125" s="5"/>
@@ -4772,11 +4792,9 @@
       <c r="W125" s="5"/>
     </row>
     <row r="126">
-      <c r="A126" s="9" t="s">
+      <c r="A126" s="14"/>
+      <c r="B126" s="10" t="s">
         <v>146</v>
-      </c>
-      <c r="B126" s="10" t="s">
-        <v>147</v>
       </c>
       <c r="C126" s="11" t="s">
         <v>7</v>
@@ -4803,9 +4821,11 @@
       <c r="W126" s="5"/>
     </row>
     <row r="127">
-      <c r="A127" s="14"/>
+      <c r="A127" s="9" t="s">
+        <v>147</v>
+      </c>
       <c r="B127" s="10" t="s">
-        <v>124</v>
+        <v>148</v>
       </c>
       <c r="C127" s="11" t="s">
         <v>7</v>
@@ -4832,16 +4852,14 @@
       <c r="W127" s="5"/>
     </row>
     <row r="128">
-      <c r="A128" s="19" t="s">
-        <v>148</v>
-      </c>
+      <c r="A128" s="13"/>
       <c r="B128" s="10" t="s">
         <v>149</v>
       </c>
       <c r="C128" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D128" s="20"/>
+      <c r="D128" s="12"/>
       <c r="E128" s="5"/>
       <c r="F128" s="5"/>
       <c r="G128" s="5"/>
@@ -4867,12 +4885,10 @@
       <c r="B129" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="C129" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D129" s="16" t="s">
-        <v>151</v>
-      </c>
+      <c r="C129" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D129" s="12"/>
       <c r="E129" s="5"/>
       <c r="F129" s="5"/>
       <c r="G129" s="5"/>
@@ -4896,7 +4912,7 @@
     <row r="130">
       <c r="A130" s="13"/>
       <c r="B130" s="10" t="s">
-        <v>152</v>
+        <v>68</v>
       </c>
       <c r="C130" s="11" t="s">
         <v>7</v>
@@ -4925,7 +4941,7 @@
     <row r="131">
       <c r="A131" s="13"/>
       <c r="B131" s="10" t="s">
-        <v>153</v>
+        <v>69</v>
       </c>
       <c r="C131" s="11" t="s">
         <v>7</v>
@@ -4954,14 +4970,12 @@
     <row r="132">
       <c r="A132" s="13"/>
       <c r="B132" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="C132" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D132" s="16" t="s">
-        <v>155</v>
-      </c>
+        <v>151</v>
+      </c>
+      <c r="C132" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D132" s="12"/>
       <c r="E132" s="5"/>
       <c r="F132" s="5"/>
       <c r="G132" s="5"/>
@@ -4985,7 +4999,7 @@
     <row r="133">
       <c r="A133" s="13"/>
       <c r="B133" s="10" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C133" s="11" t="s">
         <v>7</v>
@@ -5014,12 +5028,14 @@
     <row r="134">
       <c r="A134" s="13"/>
       <c r="B134" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="C134" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D134" s="12"/>
+        <v>153</v>
+      </c>
+      <c r="C134" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D134" s="16" t="s">
+        <v>154</v>
+      </c>
       <c r="E134" s="5"/>
       <c r="F134" s="5"/>
       <c r="G134" s="5"/>
@@ -5043,7 +5059,7 @@
     <row r="135">
       <c r="A135" s="14"/>
       <c r="B135" s="10" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C135" s="11" t="s">
         <v>7</v>
@@ -5070,12 +5086,16 @@
       <c r="W135" s="5"/>
     </row>
     <row r="136">
-      <c r="A136" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="B136" s="7"/>
-      <c r="C136" s="7"/>
-      <c r="D136" s="8"/>
+      <c r="A136" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="B136" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="C136" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D136" s="12"/>
       <c r="E136" s="5"/>
       <c r="F136" s="5"/>
       <c r="G136" s="5"/>
@@ -5097,18 +5117,14 @@
       <c r="W136" s="5"/>
     </row>
     <row r="137">
-      <c r="A137" s="9" t="s">
-        <v>160</v>
-      </c>
+      <c r="A137" s="14"/>
       <c r="B137" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="C137" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D137" s="16" t="s">
-        <v>162</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="C137" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D137" s="12"/>
       <c r="E137" s="5"/>
       <c r="F137" s="5"/>
       <c r="G137" s="5"/>
@@ -5130,16 +5146,16 @@
       <c r="W137" s="5"/>
     </row>
     <row r="138">
-      <c r="A138" s="13"/>
+      <c r="A138" s="20" t="s">
+        <v>158</v>
+      </c>
       <c r="B138" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="C138" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D138" s="16" t="s">
-        <v>164</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="C138" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D138" s="19"/>
       <c r="E138" s="5"/>
       <c r="F138" s="5"/>
       <c r="G138" s="5"/>
@@ -5161,14 +5177,16 @@
       <c r="W138" s="5"/>
     </row>
     <row r="139">
-      <c r="A139" s="14"/>
+      <c r="A139" s="13"/>
       <c r="B139" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="C139" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D139" s="12"/>
+        <v>160</v>
+      </c>
+      <c r="C139" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D139" s="16" t="s">
+        <v>154</v>
+      </c>
       <c r="E139" s="5"/>
       <c r="F139" s="5"/>
       <c r="G139" s="5"/>
@@ -5190,12 +5208,14 @@
       <c r="W139" s="5"/>
     </row>
     <row r="140">
-      <c r="A140" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="B140" s="7"/>
-      <c r="C140" s="7"/>
-      <c r="D140" s="8"/>
+      <c r="A140" s="13"/>
+      <c r="B140" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="C140" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D140" s="12"/>
       <c r="E140" s="5"/>
       <c r="F140" s="5"/>
       <c r="G140" s="5"/>
@@ -5217,11 +5237,9 @@
       <c r="W140" s="5"/>
     </row>
     <row r="141">
-      <c r="A141" s="9" t="s">
-        <v>167</v>
-      </c>
+      <c r="A141" s="13"/>
       <c r="B141" s="10" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="C141" s="11" t="s">
         <v>7</v>
@@ -5248,14 +5266,16 @@
       <c r="W141" s="5"/>
     </row>
     <row r="142">
-      <c r="A142" s="14"/>
+      <c r="A142" s="13"/>
       <c r="B142" s="10" t="s">
-        <v>169</v>
-      </c>
-      <c r="C142" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D142" s="12"/>
+        <v>163</v>
+      </c>
+      <c r="C142" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D142" s="16" t="s">
+        <v>164</v>
+      </c>
       <c r="E142" s="5"/>
       <c r="F142" s="5"/>
       <c r="G142" s="5"/>
@@ -5277,11 +5297,9 @@
       <c r="W142" s="5"/>
     </row>
     <row r="143">
-      <c r="A143" s="9" t="s">
-        <v>170</v>
-      </c>
+      <c r="A143" s="13"/>
       <c r="B143" s="10" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="C143" s="11" t="s">
         <v>7</v>
@@ -5310,7 +5328,7 @@
     <row r="144">
       <c r="A144" s="13"/>
       <c r="B144" s="10" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="C144" s="11" t="s">
         <v>7</v>
@@ -5337,9 +5355,9 @@
       <c r="W144" s="5"/>
     </row>
     <row r="145">
-      <c r="A145" s="13"/>
+      <c r="A145" s="14"/>
       <c r="B145" s="10" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="C145" s="11" t="s">
         <v>7</v>
@@ -5366,14 +5384,12 @@
       <c r="W145" s="5"/>
     </row>
     <row r="146">
-      <c r="A146" s="13"/>
-      <c r="B146" s="10" t="s">
-        <v>174</v>
-      </c>
-      <c r="C146" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D146" s="12"/>
+      <c r="A146" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="B146" s="7"/>
+      <c r="C146" s="7"/>
+      <c r="D146" s="8"/>
       <c r="E146" s="5"/>
       <c r="F146" s="5"/>
       <c r="G146" s="5"/>
@@ -5395,14 +5411,18 @@
       <c r="W146" s="5"/>
     </row>
     <row r="147">
-      <c r="A147" s="13"/>
+      <c r="A147" s="9" t="s">
+        <v>169</v>
+      </c>
       <c r="B147" s="10" t="s">
-        <v>175</v>
-      </c>
-      <c r="C147" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D147" s="12"/>
+        <v>170</v>
+      </c>
+      <c r="C147" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D147" s="16" t="s">
+        <v>171</v>
+      </c>
       <c r="E147" s="5"/>
       <c r="F147" s="5"/>
       <c r="G147" s="5"/>
@@ -5426,12 +5446,14 @@
     <row r="148">
       <c r="A148" s="13"/>
       <c r="B148" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="C148" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D148" s="12"/>
+        <v>172</v>
+      </c>
+      <c r="C148" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D148" s="16" t="s">
+        <v>173</v>
+      </c>
       <c r="E148" s="5"/>
       <c r="F148" s="5"/>
       <c r="G148" s="5"/>
@@ -5453,9 +5475,9 @@
       <c r="W148" s="5"/>
     </row>
     <row r="149">
-      <c r="A149" s="13"/>
+      <c r="A149" s="14"/>
       <c r="B149" s="10" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C149" s="11" t="s">
         <v>7</v>
@@ -5482,14 +5504,12 @@
       <c r="W149" s="5"/>
     </row>
     <row r="150">
-      <c r="A150" s="13"/>
-      <c r="B150" s="21" t="s">
-        <v>178</v>
-      </c>
-      <c r="C150" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D150" s="12"/>
+      <c r="A150" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="B150" s="7"/>
+      <c r="C150" s="7"/>
+      <c r="D150" s="8"/>
       <c r="E150" s="5"/>
       <c r="F150" s="5"/>
       <c r="G150" s="5"/>
@@ -5511,9 +5531,11 @@
       <c r="W150" s="5"/>
     </row>
     <row r="151">
-      <c r="A151" s="13"/>
-      <c r="B151" s="21" t="s">
-        <v>179</v>
+      <c r="A151" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="B151" s="10" t="s">
+        <v>177</v>
       </c>
       <c r="C151" s="11" t="s">
         <v>7</v>
@@ -5540,9 +5562,9 @@
       <c r="W151" s="5"/>
     </row>
     <row r="152">
-      <c r="A152" s="13"/>
-      <c r="B152" s="21" t="s">
-        <v>180</v>
+      <c r="A152" s="14"/>
+      <c r="B152" s="10" t="s">
+        <v>178</v>
       </c>
       <c r="C152" s="11" t="s">
         <v>7</v>
@@ -5569,16 +5591,16 @@
       <c r="W152" s="5"/>
     </row>
     <row r="153">
-      <c r="A153" s="13"/>
-      <c r="B153" s="21" t="s">
-        <v>181</v>
-      </c>
-      <c r="C153" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D153" s="16" t="s">
-        <v>182</v>
-      </c>
+      <c r="A153" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="B153" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="C153" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D153" s="12"/>
       <c r="E153" s="5"/>
       <c r="F153" s="5"/>
       <c r="G153" s="5"/>
@@ -5601,8 +5623,8 @@
     </row>
     <row r="154">
       <c r="A154" s="13"/>
-      <c r="B154" s="21" t="s">
-        <v>183</v>
+      <c r="B154" s="10" t="s">
+        <v>181</v>
       </c>
       <c r="C154" s="11" t="s">
         <v>7</v>
@@ -5629,9 +5651,9 @@
       <c r="W154" s="5"/>
     </row>
     <row r="155">
-      <c r="A155" s="14"/>
-      <c r="B155" s="21" t="s">
-        <v>184</v>
+      <c r="A155" s="13"/>
+      <c r="B155" s="10" t="s">
+        <v>182</v>
       </c>
       <c r="C155" s="11" t="s">
         <v>7</v>
@@ -5658,14 +5680,14 @@
       <c r="W155" s="5"/>
     </row>
     <row r="156">
-      <c r="A156" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="B156" s="22" t="s">
-        <v>186</v>
-      </c>
-      <c r="C156" s="7"/>
-      <c r="D156" s="8"/>
+      <c r="A156" s="13"/>
+      <c r="B156" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="C156" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D156" s="12"/>
       <c r="E156" s="5"/>
       <c r="F156" s="5"/>
       <c r="G156" s="5"/>
@@ -5689,7 +5711,7 @@
     <row r="157">
       <c r="A157" s="13"/>
       <c r="B157" s="10" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C157" s="11" t="s">
         <v>7</v>
@@ -5718,7 +5740,7 @@
     <row r="158">
       <c r="A158" s="13"/>
       <c r="B158" s="10" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C158" s="11" t="s">
         <v>7</v>
@@ -5747,7 +5769,7 @@
     <row r="159">
       <c r="A159" s="13"/>
       <c r="B159" s="10" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C159" s="11" t="s">
         <v>7</v>
@@ -5775,8 +5797,8 @@
     </row>
     <row r="160">
       <c r="A160" s="13"/>
-      <c r="B160" s="10" t="s">
-        <v>190</v>
+      <c r="B160" s="21" t="s">
+        <v>187</v>
       </c>
       <c r="C160" s="11" t="s">
         <v>7</v>
@@ -5804,8 +5826,8 @@
     </row>
     <row r="161">
       <c r="A161" s="13"/>
-      <c r="B161" s="10" t="s">
-        <v>191</v>
+      <c r="B161" s="21" t="s">
+        <v>188</v>
       </c>
       <c r="C161" s="11" t="s">
         <v>7</v>
@@ -5833,8 +5855,8 @@
     </row>
     <row r="162">
       <c r="A162" s="13"/>
-      <c r="B162" s="10" t="s">
-        <v>192</v>
+      <c r="B162" s="21" t="s">
+        <v>189</v>
       </c>
       <c r="C162" s="11" t="s">
         <v>7</v>
@@ -5862,13 +5884,15 @@
     </row>
     <row r="163">
       <c r="A163" s="13"/>
-      <c r="B163" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="C163" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D163" s="12"/>
+      <c r="B163" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="C163" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D163" s="16" t="s">
+        <v>191</v>
+      </c>
       <c r="E163" s="5"/>
       <c r="F163" s="5"/>
       <c r="G163" s="5"/>
@@ -5891,8 +5915,8 @@
     </row>
     <row r="164">
       <c r="A164" s="13"/>
-      <c r="B164" s="10" t="s">
-        <v>194</v>
+      <c r="B164" s="21" t="s">
+        <v>192</v>
       </c>
       <c r="C164" s="11" t="s">
         <v>7</v>
@@ -5919,9 +5943,9 @@
       <c r="W164" s="5"/>
     </row>
     <row r="165">
-      <c r="A165" s="13"/>
+      <c r="A165" s="14"/>
       <c r="B165" s="21" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C165" s="11" t="s">
         <v>7</v>
@@ -5948,16 +5972,14 @@
       <c r="W165" s="5"/>
     </row>
     <row r="166">
-      <c r="A166" s="13"/>
-      <c r="B166" s="21" t="s">
-        <v>196</v>
-      </c>
-      <c r="C166" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="D166" s="24" t="s">
-        <v>197</v>
-      </c>
+      <c r="A166" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="B166" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="C166" s="7"/>
+      <c r="D166" s="8"/>
       <c r="E166" s="5"/>
       <c r="F166" s="5"/>
       <c r="G166" s="5"/>
@@ -5979,14 +6001,14 @@
       <c r="W166" s="5"/>
     </row>
     <row r="167">
-      <c r="A167" s="14"/>
-      <c r="B167" s="21" t="s">
-        <v>198</v>
+      <c r="A167" s="13"/>
+      <c r="B167" s="10" t="s">
+        <v>196</v>
       </c>
       <c r="C167" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D167" s="24"/>
+      <c r="D167" s="12"/>
       <c r="E167" s="5"/>
       <c r="F167" s="5"/>
       <c r="G167" s="5"/>
@@ -6008,10 +6030,14 @@
       <c r="W167" s="5"/>
     </row>
     <row r="168">
-      <c r="A168" s="5"/>
-      <c r="B168" s="5"/>
-      <c r="C168" s="5"/>
-      <c r="D168" s="5"/>
+      <c r="A168" s="13"/>
+      <c r="B168" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="C168" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D168" s="12"/>
       <c r="E168" s="5"/>
       <c r="F168" s="5"/>
       <c r="G168" s="5"/>
@@ -6033,10 +6059,14 @@
       <c r="W168" s="5"/>
     </row>
     <row r="169">
-      <c r="A169" s="5"/>
-      <c r="B169" s="5"/>
-      <c r="C169" s="5"/>
-      <c r="D169" s="5"/>
+      <c r="A169" s="13"/>
+      <c r="B169" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="C169" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D169" s="12"/>
       <c r="E169" s="5"/>
       <c r="F169" s="5"/>
       <c r="G169" s="5"/>
@@ -6058,10 +6088,14 @@
       <c r="W169" s="5"/>
     </row>
     <row r="170">
-      <c r="A170" s="5"/>
-      <c r="B170" s="5"/>
-      <c r="C170" s="5"/>
-      <c r="D170" s="5"/>
+      <c r="A170" s="13"/>
+      <c r="B170" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="C170" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D170" s="12"/>
       <c r="E170" s="5"/>
       <c r="F170" s="5"/>
       <c r="G170" s="5"/>
@@ -6083,10 +6117,14 @@
       <c r="W170" s="5"/>
     </row>
     <row r="171">
-      <c r="A171" s="5"/>
-      <c r="B171" s="5"/>
-      <c r="C171" s="5"/>
-      <c r="D171" s="5"/>
+      <c r="A171" s="13"/>
+      <c r="B171" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="C171" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D171" s="12"/>
       <c r="E171" s="5"/>
       <c r="F171" s="5"/>
       <c r="G171" s="5"/>
@@ -6108,10 +6146,14 @@
       <c r="W171" s="5"/>
     </row>
     <row r="172">
-      <c r="A172" s="5"/>
-      <c r="B172" s="5"/>
-      <c r="C172" s="5"/>
-      <c r="D172" s="5"/>
+      <c r="A172" s="13"/>
+      <c r="B172" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="C172" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D172" s="12"/>
       <c r="E172" s="5"/>
       <c r="F172" s="5"/>
       <c r="G172" s="5"/>
@@ -6133,10 +6175,14 @@
       <c r="W172" s="5"/>
     </row>
     <row r="173">
-      <c r="A173" s="5"/>
-      <c r="B173" s="5"/>
-      <c r="C173" s="5"/>
-      <c r="D173" s="5"/>
+      <c r="A173" s="13"/>
+      <c r="B173" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="C173" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D173" s="12"/>
       <c r="E173" s="5"/>
       <c r="F173" s="5"/>
       <c r="G173" s="5"/>
@@ -6158,10 +6204,14 @@
       <c r="W173" s="5"/>
     </row>
     <row r="174">
-      <c r="A174" s="5"/>
-      <c r="B174" s="5"/>
-      <c r="C174" s="5"/>
-      <c r="D174" s="5"/>
+      <c r="A174" s="13"/>
+      <c r="B174" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="C174" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D174" s="12"/>
       <c r="E174" s="5"/>
       <c r="F174" s="5"/>
       <c r="G174" s="5"/>
@@ -6183,10 +6233,14 @@
       <c r="W174" s="5"/>
     </row>
     <row r="175">
-      <c r="A175" s="5"/>
-      <c r="B175" s="5"/>
-      <c r="C175" s="5"/>
-      <c r="D175" s="5"/>
+      <c r="A175" s="13"/>
+      <c r="B175" s="21" t="s">
+        <v>204</v>
+      </c>
+      <c r="C175" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D175" s="12"/>
       <c r="E175" s="5"/>
       <c r="F175" s="5"/>
       <c r="G175" s="5"/>
@@ -6208,10 +6262,16 @@
       <c r="W175" s="5"/>
     </row>
     <row r="176">
-      <c r="A176" s="5"/>
-      <c r="B176" s="5"/>
-      <c r="C176" s="5"/>
-      <c r="D176" s="5"/>
+      <c r="A176" s="13"/>
+      <c r="B176" s="21" t="s">
+        <v>205</v>
+      </c>
+      <c r="C176" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D176" s="16" t="s">
+        <v>206</v>
+      </c>
       <c r="E176" s="5"/>
       <c r="F176" s="5"/>
       <c r="G176" s="5"/>
@@ -6233,10 +6293,14 @@
       <c r="W176" s="5"/>
     </row>
     <row r="177">
-      <c r="A177" s="5"/>
-      <c r="B177" s="5"/>
-      <c r="C177" s="5"/>
-      <c r="D177" s="5"/>
+      <c r="A177" s="14"/>
+      <c r="B177" s="21" t="s">
+        <v>207</v>
+      </c>
+      <c r="C177" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D177" s="23"/>
       <c r="E177" s="5"/>
       <c r="F177" s="5"/>
       <c r="G177" s="5"/>
@@ -25257,8 +25321,258 @@
       <c r="V937" s="5"/>
       <c r="W937" s="5"/>
     </row>
+    <row r="938">
+      <c r="A938" s="5"/>
+      <c r="B938" s="5"/>
+      <c r="C938" s="5"/>
+      <c r="D938" s="5"/>
+      <c r="E938" s="5"/>
+      <c r="F938" s="5"/>
+      <c r="G938" s="5"/>
+      <c r="H938" s="5"/>
+      <c r="I938" s="5"/>
+      <c r="J938" s="5"/>
+      <c r="K938" s="5"/>
+      <c r="L938" s="5"/>
+      <c r="M938" s="5"/>
+      <c r="N938" s="5"/>
+      <c r="O938" s="5"/>
+      <c r="P938" s="5"/>
+      <c r="Q938" s="5"/>
+      <c r="R938" s="5"/>
+      <c r="S938" s="5"/>
+      <c r="T938" s="5"/>
+      <c r="U938" s="5"/>
+      <c r="V938" s="5"/>
+      <c r="W938" s="5"/>
+    </row>
+    <row r="939">
+      <c r="A939" s="5"/>
+      <c r="B939" s="5"/>
+      <c r="C939" s="5"/>
+      <c r="D939" s="5"/>
+      <c r="E939" s="5"/>
+      <c r="F939" s="5"/>
+      <c r="G939" s="5"/>
+      <c r="H939" s="5"/>
+      <c r="I939" s="5"/>
+      <c r="J939" s="5"/>
+      <c r="K939" s="5"/>
+      <c r="L939" s="5"/>
+      <c r="M939" s="5"/>
+      <c r="N939" s="5"/>
+      <c r="O939" s="5"/>
+      <c r="P939" s="5"/>
+      <c r="Q939" s="5"/>
+      <c r="R939" s="5"/>
+      <c r="S939" s="5"/>
+      <c r="T939" s="5"/>
+      <c r="U939" s="5"/>
+      <c r="V939" s="5"/>
+      <c r="W939" s="5"/>
+    </row>
+    <row r="940">
+      <c r="A940" s="5"/>
+      <c r="B940" s="5"/>
+      <c r="C940" s="5"/>
+      <c r="D940" s="5"/>
+      <c r="E940" s="5"/>
+      <c r="F940" s="5"/>
+      <c r="G940" s="5"/>
+      <c r="H940" s="5"/>
+      <c r="I940" s="5"/>
+      <c r="J940" s="5"/>
+      <c r="K940" s="5"/>
+      <c r="L940" s="5"/>
+      <c r="M940" s="5"/>
+      <c r="N940" s="5"/>
+      <c r="O940" s="5"/>
+      <c r="P940" s="5"/>
+      <c r="Q940" s="5"/>
+      <c r="R940" s="5"/>
+      <c r="S940" s="5"/>
+      <c r="T940" s="5"/>
+      <c r="U940" s="5"/>
+      <c r="V940" s="5"/>
+      <c r="W940" s="5"/>
+    </row>
+    <row r="941">
+      <c r="A941" s="5"/>
+      <c r="B941" s="5"/>
+      <c r="C941" s="5"/>
+      <c r="D941" s="5"/>
+      <c r="E941" s="5"/>
+      <c r="F941" s="5"/>
+      <c r="G941" s="5"/>
+      <c r="H941" s="5"/>
+      <c r="I941" s="5"/>
+      <c r="J941" s="5"/>
+      <c r="K941" s="5"/>
+      <c r="L941" s="5"/>
+      <c r="M941" s="5"/>
+      <c r="N941" s="5"/>
+      <c r="O941" s="5"/>
+      <c r="P941" s="5"/>
+      <c r="Q941" s="5"/>
+      <c r="R941" s="5"/>
+      <c r="S941" s="5"/>
+      <c r="T941" s="5"/>
+      <c r="U941" s="5"/>
+      <c r="V941" s="5"/>
+      <c r="W941" s="5"/>
+    </row>
+    <row r="942">
+      <c r="A942" s="5"/>
+      <c r="B942" s="5"/>
+      <c r="C942" s="5"/>
+      <c r="D942" s="5"/>
+      <c r="E942" s="5"/>
+      <c r="F942" s="5"/>
+      <c r="G942" s="5"/>
+      <c r="H942" s="5"/>
+      <c r="I942" s="5"/>
+      <c r="J942" s="5"/>
+      <c r="K942" s="5"/>
+      <c r="L942" s="5"/>
+      <c r="M942" s="5"/>
+      <c r="N942" s="5"/>
+      <c r="O942" s="5"/>
+      <c r="P942" s="5"/>
+      <c r="Q942" s="5"/>
+      <c r="R942" s="5"/>
+      <c r="S942" s="5"/>
+      <c r="T942" s="5"/>
+      <c r="U942" s="5"/>
+      <c r="V942" s="5"/>
+      <c r="W942" s="5"/>
+    </row>
+    <row r="943">
+      <c r="A943" s="5"/>
+      <c r="B943" s="5"/>
+      <c r="C943" s="5"/>
+      <c r="D943" s="5"/>
+      <c r="E943" s="5"/>
+      <c r="F943" s="5"/>
+      <c r="G943" s="5"/>
+      <c r="H943" s="5"/>
+      <c r="I943" s="5"/>
+      <c r="J943" s="5"/>
+      <c r="K943" s="5"/>
+      <c r="L943" s="5"/>
+      <c r="M943" s="5"/>
+      <c r="N943" s="5"/>
+      <c r="O943" s="5"/>
+      <c r="P943" s="5"/>
+      <c r="Q943" s="5"/>
+      <c r="R943" s="5"/>
+      <c r="S943" s="5"/>
+      <c r="T943" s="5"/>
+      <c r="U943" s="5"/>
+      <c r="V943" s="5"/>
+      <c r="W943" s="5"/>
+    </row>
+    <row r="944">
+      <c r="A944" s="5"/>
+      <c r="B944" s="5"/>
+      <c r="C944" s="5"/>
+      <c r="D944" s="5"/>
+      <c r="E944" s="5"/>
+      <c r="F944" s="5"/>
+      <c r="G944" s="5"/>
+      <c r="H944" s="5"/>
+      <c r="I944" s="5"/>
+      <c r="J944" s="5"/>
+      <c r="K944" s="5"/>
+      <c r="L944" s="5"/>
+      <c r="M944" s="5"/>
+      <c r="N944" s="5"/>
+      <c r="O944" s="5"/>
+      <c r="P944" s="5"/>
+      <c r="Q944" s="5"/>
+      <c r="R944" s="5"/>
+      <c r="S944" s="5"/>
+      <c r="T944" s="5"/>
+      <c r="U944" s="5"/>
+      <c r="V944" s="5"/>
+      <c r="W944" s="5"/>
+    </row>
+    <row r="945">
+      <c r="A945" s="5"/>
+      <c r="B945" s="5"/>
+      <c r="C945" s="5"/>
+      <c r="D945" s="5"/>
+      <c r="E945" s="5"/>
+      <c r="F945" s="5"/>
+      <c r="G945" s="5"/>
+      <c r="H945" s="5"/>
+      <c r="I945" s="5"/>
+      <c r="J945" s="5"/>
+      <c r="K945" s="5"/>
+      <c r="L945" s="5"/>
+      <c r="M945" s="5"/>
+      <c r="N945" s="5"/>
+      <c r="O945" s="5"/>
+      <c r="P945" s="5"/>
+      <c r="Q945" s="5"/>
+      <c r="R945" s="5"/>
+      <c r="S945" s="5"/>
+      <c r="T945" s="5"/>
+      <c r="U945" s="5"/>
+      <c r="V945" s="5"/>
+      <c r="W945" s="5"/>
+    </row>
+    <row r="946">
+      <c r="A946" s="5"/>
+      <c r="B946" s="5"/>
+      <c r="C946" s="5"/>
+      <c r="D946" s="5"/>
+      <c r="E946" s="5"/>
+      <c r="F946" s="5"/>
+      <c r="G946" s="5"/>
+      <c r="H946" s="5"/>
+      <c r="I946" s="5"/>
+      <c r="J946" s="5"/>
+      <c r="K946" s="5"/>
+      <c r="L946" s="5"/>
+      <c r="M946" s="5"/>
+      <c r="N946" s="5"/>
+      <c r="O946" s="5"/>
+      <c r="P946" s="5"/>
+      <c r="Q946" s="5"/>
+      <c r="R946" s="5"/>
+      <c r="S946" s="5"/>
+      <c r="T946" s="5"/>
+      <c r="U946" s="5"/>
+      <c r="V946" s="5"/>
+      <c r="W946" s="5"/>
+    </row>
+    <row r="947">
+      <c r="A947" s="5"/>
+      <c r="B947" s="5"/>
+      <c r="C947" s="5"/>
+      <c r="D947" s="5"/>
+      <c r="E947" s="5"/>
+      <c r="F947" s="5"/>
+      <c r="G947" s="5"/>
+      <c r="H947" s="5"/>
+      <c r="I947" s="5"/>
+      <c r="J947" s="5"/>
+      <c r="K947" s="5"/>
+      <c r="L947" s="5"/>
+      <c r="M947" s="5"/>
+      <c r="N947" s="5"/>
+      <c r="O947" s="5"/>
+      <c r="P947" s="5"/>
+      <c r="Q947" s="5"/>
+      <c r="R947" s="5"/>
+      <c r="S947" s="5"/>
+      <c r="T947" s="5"/>
+      <c r="U947" s="5"/>
+      <c r="V947" s="5"/>
+      <c r="W947" s="5"/>
+    </row>
   </sheetData>
-  <mergeCells count="31">
+  <mergeCells count="32">
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A9"/>
@@ -25275,24 +25589,25 @@
     <mergeCell ref="A52:A57"/>
     <mergeCell ref="A58:A66"/>
     <mergeCell ref="A67:A68"/>
-    <mergeCell ref="A69:A87"/>
-    <mergeCell ref="A88:D88"/>
-    <mergeCell ref="A89:A92"/>
-    <mergeCell ref="A93:A99"/>
-    <mergeCell ref="A100:A112"/>
-    <mergeCell ref="A143:A155"/>
-    <mergeCell ref="A156:A167"/>
-    <mergeCell ref="A113:A125"/>
-    <mergeCell ref="A126:A127"/>
-    <mergeCell ref="A128:A135"/>
-    <mergeCell ref="A136:D136"/>
-    <mergeCell ref="A137:A139"/>
-    <mergeCell ref="A140:D140"/>
-    <mergeCell ref="A141:A142"/>
-    <mergeCell ref="B156:D156"/>
+    <mergeCell ref="A69:A88"/>
+    <mergeCell ref="A89:D89"/>
+    <mergeCell ref="A90:A93"/>
+    <mergeCell ref="A94:A100"/>
+    <mergeCell ref="A101:A113"/>
+    <mergeCell ref="A151:A152"/>
+    <mergeCell ref="A153:A165"/>
+    <mergeCell ref="A166:A177"/>
+    <mergeCell ref="A114:A126"/>
+    <mergeCell ref="A127:A135"/>
+    <mergeCell ref="A136:A137"/>
+    <mergeCell ref="A138:A145"/>
+    <mergeCell ref="A146:D146"/>
+    <mergeCell ref="A147:A149"/>
+    <mergeCell ref="A150:D150"/>
+    <mergeCell ref="B166:D166"/>
   </mergeCells>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="C3:C9 C11:C25 C27 C29:C87 C89:C135 C137:C139 C141:C155 C157:C167">
+    <dataValidation type="list" allowBlank="1" sqref="C3:C9 C11:C25 C27 C29:C88 C90:C145 C147:C149 C151:C165 C167:C177">
       <formula1>"Passed,Failed,Scipped"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Tests, check and test cases updated
</commit_message>
<xml_diff>
--- a/Documentation/Check.xlsx
+++ b/Documentation/Check.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="208">
   <si>
     <t>Группа проверок/модуль</t>
   </si>
@@ -865,11 +865,11 @@
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="6" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
@@ -4020,10 +4020,12 @@
       <c r="B100" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="C100" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D100" s="19"/>
+      <c r="C100" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D100" s="16" t="s">
+        <v>109</v>
+      </c>
       <c r="E100" s="5"/>
       <c r="F100" s="5"/>
       <c r="G100" s="5"/>
@@ -5146,7 +5148,7 @@
       <c r="W137" s="5"/>
     </row>
     <row r="138">
-      <c r="A138" s="20" t="s">
+      <c r="A138" s="19" t="s">
         <v>158</v>
       </c>
       <c r="B138" s="10" t="s">
@@ -5155,7 +5157,7 @@
       <c r="C138" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D138" s="19"/>
+      <c r="D138" s="20"/>
       <c r="E138" s="5"/>
       <c r="F138" s="5"/>
       <c r="G138" s="5"/>

</xml_diff>